<commit_message>
add res boundary attack for SEED 88
</commit_message>
<xml_diff>
--- a/results/birth/SEED_88/result.xlsx
+++ b/results/birth/SEED_88/result.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ12"/>
+  <dimension ref="A1:AR12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,6 +546,18 @@
       <c r="AH1" s="1" t="n"/>
       <c r="AI1" s="1" t="n"/>
       <c r="AJ1" s="1" t="n"/>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>BOUNDARY</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="n"/>
+      <c r="AM1" s="1" t="n"/>
+      <c r="AN1" s="1" t="n"/>
+      <c r="AO1" s="1" t="n"/>
+      <c r="AP1" s="1" t="n"/>
+      <c r="AQ1" s="1" t="n"/>
+      <c r="AR1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="B2" s="1" t="inlineStr">
@@ -723,6 +735,46 @@
           <t>0.20</t>
         </is>
       </c>
+      <c r="AK2" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="AL2" s="1" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="AM2" s="1" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="AN2" s="1" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
+      <c r="AO2" s="1" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="AP2" s="1" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="AQ2" s="1" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="AR2" s="1" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -848,6 +900,30 @@
       </c>
       <c r="AJ4" t="n">
         <v>2029.032592455546</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>390.3992577044169</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>391.8017908287048</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>398.8038006528218</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>401.2359029515584</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>421.3227803293864</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>437.3160461616516</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>463.2117540168762</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>651.9611461575826</v>
       </c>
     </row>
     <row r="5">
@@ -959,6 +1035,30 @@
       <c r="AJ5" t="n">
         <v>2092.501782380617</v>
       </c>
+      <c r="AK5" t="n">
+        <v>489.2113279360275</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>491.5688788238218</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>494.9450467217215</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>497.7337667428206</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>530.339194723864</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>554.1363678360606</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>567.5598559118322</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>818.6349930379963</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
@@ -977,7 +1077,7 @@
         <v>0.9990971437455756</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9990687356509987</v>
+        <v>0.9990687356509985</v>
       </c>
       <c r="G6" t="n">
         <v>0.9990818133784113</v>
@@ -989,10 +1089,10 @@
         <v>0.9990383888537845</v>
       </c>
       <c r="J6" t="n">
-        <v>0.9990089146365941</v>
+        <v>0.9990089146365944</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9989420615148384</v>
+        <v>0.9989420615148382</v>
       </c>
       <c r="L6" t="n">
         <v>0.9982414008436371</v>
@@ -1001,7 +1101,7 @@
         <v>0.9990936914796713</v>
       </c>
       <c r="N6" t="n">
-        <v>0.999082239761055</v>
+        <v>0.9990822397610548</v>
       </c>
       <c r="O6" t="n">
         <v>0.9990826455373331</v>
@@ -1013,10 +1113,10 @@
         <v>0.9990897145465298</v>
       </c>
       <c r="R6" t="n">
-        <v>0.9990747589810027</v>
+        <v>0.9990747589810025</v>
       </c>
       <c r="S6" t="n">
-        <v>0.9990665717275091</v>
+        <v>0.9990665717275093</v>
       </c>
       <c r="T6" t="n">
         <v>0.9988866227428247</v>
@@ -1028,13 +1128,13 @@
         <v>0.9985081409694726</v>
       </c>
       <c r="W6" t="n">
-        <v>0.9981172722701454</v>
+        <v>0.9981172722701451</v>
       </c>
       <c r="X6" t="n">
         <v>0.9977150028221838</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.9971664375423133</v>
+        <v>0.9971664375423135</v>
       </c>
       <c r="Z6" t="n">
         <v>0.99573219035195</v>
@@ -1046,13 +1146,13 @@
         <v>0.9841573065711861</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.9987903087061288</v>
+        <v>0.9987903087061284</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.9984271428906178</v>
+        <v>0.9984271428906181</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.9979740729933867</v>
+        <v>0.9979740729933866</v>
       </c>
       <c r="AF6" t="n">
         <v>0.9975081378455098</v>
@@ -1064,10 +1164,34 @@
         <v>0.9952122099461452</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.9932168311616114</v>
+        <v>0.9932168311616112</v>
       </c>
       <c r="AJ6" t="n">
         <v>0.9832105121811606</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>0.9990755579861272</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>0.9990673890700759</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>0.9990557359144541</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>0.9990432672346851</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>0.9989105669777159</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>0.9988262245787846</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>0.9987713311790573</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>0.9975022087184466</v>
       </c>
     </row>
     <row r="7">
@@ -1182,6 +1306,30 @@
       </c>
       <c r="AJ7" t="n">
         <v>2026.610440700849</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>537.1415200042725</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>540.281365292867</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>541.9926981226603</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>555.7811170260112</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>558.6827701505025</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>571.9447099622091</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>595.4838717969259</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>775.259315624237</v>
       </c>
     </row>
     <row r="8">
@@ -1293,6 +1441,30 @@
       <c r="AJ8" t="n">
         <v>2077.69059578045</v>
       </c>
+      <c r="AK8" t="n">
+        <v>649.671967341643</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>653.7355689588217</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>658.1318471867484</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>678.5656354234328</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>673.1440240242024</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>694.3897178746944</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>717.6490616161614</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>927.8302652424078</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
@@ -1308,7 +1480,7 @@
         <v>0.9992459475793259</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9990202767977289</v>
+        <v>0.9990202767977286</v>
       </c>
       <c r="F9" t="n">
         <v>0.9989516748313217</v>
@@ -1320,7 +1492,7 @@
         <v>0.9987708602376143</v>
       </c>
       <c r="I9" t="n">
-        <v>0.9986559571695054</v>
+        <v>0.9986559571695052</v>
       </c>
       <c r="J9" t="n">
         <v>0.9982814469900476</v>
@@ -1332,7 +1504,7 @@
         <v>0.9937570884782422</v>
       </c>
       <c r="M9" t="n">
-        <v>0.9990202767977289</v>
+        <v>0.9990202767977286</v>
       </c>
       <c r="N9" t="n">
         <v>0.9989534512175199</v>
@@ -1341,7 +1513,7 @@
         <v>0.9988816561076274</v>
       </c>
       <c r="P9" t="n">
-        <v>0.9987956391672494</v>
+        <v>0.9987956391672492</v>
       </c>
       <c r="Q9" t="n">
         <v>0.9986925929506112</v>
@@ -1356,10 +1528,10 @@
         <v>0.9949140761597574</v>
       </c>
       <c r="U9" t="n">
-        <v>0.9989322763309331</v>
+        <v>0.9989322763309333</v>
       </c>
       <c r="V9" t="n">
-        <v>0.9987562371960801</v>
+        <v>0.9987562371960799</v>
       </c>
       <c r="W9" t="n">
         <v>0.9985436327254189</v>
@@ -1380,19 +1552,19 @@
         <v>0.9878153984722536</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.9988943855504205</v>
+        <v>0.9988943855504203</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.9986661050700375</v>
+        <v>0.9986661050700377</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.9983825694895387</v>
+        <v>0.9983825694895385</v>
       </c>
       <c r="AF9" t="n">
         <v>0.9980358622135678</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.9976122245473197</v>
+        <v>0.9976122245473198</v>
       </c>
       <c r="AH9" t="n">
         <v>0.9961605429974177</v>
@@ -1402,6 +1574,30 @@
       </c>
       <c r="AJ9" t="n">
         <v>0.9849975356038644</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>0.9990671685500947</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>0.9990470537408496</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>0.9990643617599748</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>0.9989418088728429</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>0.9989692877497833</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>0.9988450356825828</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>0.9986796817364582</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>0.9972872214855639</v>
       </c>
     </row>
     <row r="10">
@@ -1516,6 +1712,30 @@
       </c>
       <c r="AJ10" t="n">
         <v>1840.09802423954</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>310.8977380053202</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>315.2886210187276</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>320.1887220573425</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>323.6158444023133</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>335.4404909070333</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>382.5507218424479</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>409.1945012728373</v>
+      </c>
+      <c r="AR10" t="n">
+        <v>676.986574529012</v>
       </c>
     </row>
     <row r="11">
@@ -1627,6 +1847,30 @@
       <c r="AJ11" t="n">
         <v>1908.438950697823</v>
       </c>
+      <c r="AK11" t="n">
+        <v>428.7031259102286</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>431.3301281492065</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>435.3153895389307</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>439.1204777305023</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>448.764046995636</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>509.2524243842903</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>528.005104241012</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>885.9279588019787</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
@@ -1636,10 +1880,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.9993477063791678</v>
+        <v>0.9993477063791676</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9992374683335242</v>
+        <v>0.999237468333524</v>
       </c>
       <c r="E12" t="n">
         <v>0.9990633648098646</v>
@@ -1675,13 +1919,13 @@
         <v>0.9992771170036132</v>
       </c>
       <c r="P12" t="n">
-        <v>0.9992314012229798</v>
+        <v>0.9992314012229793</v>
       </c>
       <c r="Q12" t="n">
         <v>0.9991787976269871</v>
       </c>
       <c r="R12" t="n">
-        <v>0.9990714537975355</v>
+        <v>0.9990714537975353</v>
       </c>
       <c r="S12" t="n">
         <v>0.9988478935052868</v>
@@ -1699,16 +1943,16 @@
         <v>0.9987366090709446</v>
       </c>
       <c r="X12" t="n">
-        <v>0.9984518659263648</v>
+        <v>0.9984518659263646</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.9981222684962209</v>
+        <v>0.9981222684962211</v>
       </c>
       <c r="Z12" t="n">
         <v>0.9970690480045936</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.9955996452858142</v>
+        <v>0.995599645285814</v>
       </c>
       <c r="AB12" t="n">
         <v>0.9862034481672269</v>
@@ -1720,7 +1964,7 @@
         <v>0.9988967765922554</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.9985937376995944</v>
+        <v>0.9985937376995941</v>
       </c>
       <c r="AF12" t="n">
         <v>0.9982382137102586</v>
@@ -1737,15 +1981,40 @@
       <c r="AJ12" t="n">
         <v>0.9862208494609601</v>
       </c>
+      <c r="AK12" t="n">
+        <v>0.9993372423833846</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>0.9993306313821481</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>0.9993179189799252</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>0.9993042057978951</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>0.9992698019827521</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>0.9990401874922721</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>0.9989535001256086</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>0.9969671125511961</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="M1:T1"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="E1:L1"/>
     <mergeCell ref="AC1:AJ1"/>
+    <mergeCell ref="AK1:AR1"/>
     <mergeCell ref="U1:AB1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>